<commit_message>
Intial files from dell laptop
</commit_message>
<xml_diff>
--- a/prior_probabilities.xlsx
+++ b/prior_probabilities.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\origin\Desktop\Gesture5GHzDemo\gesture_tracking\conditional_probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866AD74-A6C1-445A-A082-5C77AAEF9B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9578E8-6760-43BF-B1DF-6C5B4D6D8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="2" xr2:uid="{1B4D7DD2-FA13-4C63-AFCD-7538AF6D1B2F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="4" xr2:uid="{1B4D7DD2-FA13-4C63-AFCD-7538AF6D1B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Prior" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
     <sheet name="AnglePrior" sheetId="3" r:id="rId3"/>
-    <sheet name="MPrior" sheetId="4" r:id="rId4"/>
+    <sheet name="AnglePrior4" sheetId="5" r:id="rId4"/>
+    <sheet name="MPrior4" sheetId="6" r:id="rId5"/>
+    <sheet name="MPrior" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
     <t>Character</t>
   </si>
@@ -207,6 +209,36 @@
   </si>
   <si>
     <t>seg3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = z, a2 = z, a3 = z    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = z, a2 = z, a3 = a    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = z, a2 = a, a3 = z    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = z, a2 = a, a3 = a    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = a, a2 = z, a3 = z    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = a, a2 = z, a3 = a    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = a, a2 = a, a3 = z    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a1 = a, a2 = a, a3 = a    </t>
+  </si>
+  <si>
+    <t>seg4</t>
+  </si>
+  <si>
+    <t>seg2</t>
   </si>
 </sst>
 </file>
@@ -1882,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3CB557-8655-4F16-8132-CF228E3971CF}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2020,11 +2052,373 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAC62DF-F71C-420B-8B8A-6766BAC94FC5}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="6" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J14" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C260D1D8-DD7A-4591-9F99-B58043F5F07A}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="9.06640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7BABA2-EF4C-498B-B0B8-4502078A7634}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
basic working version with angle pdf
</commit_message>
<xml_diff>
--- a/prior_probabilities.xlsx
+++ b/prior_probabilities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\origin\Desktop\Gesture5GHzDemo\gesture_tracking\conditional_probability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WiCode\conditional_probability_gesture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9578E8-6760-43BF-B1DF-6C5B4D6D8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E19CB-4654-4F3A-9660-EC4DE003AD81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="4" xr2:uid="{1B4D7DD2-FA13-4C63-AFCD-7538AF6D1B2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{1B4D7DD2-FA13-4C63-AFCD-7538AF6D1B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Prior" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="AnglePrior4" sheetId="5" r:id="rId4"/>
     <sheet name="MPrior4" sheetId="6" r:id="rId5"/>
     <sheet name="MPrior" sheetId="4" r:id="rId6"/>
+    <sheet name="3segment" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>Character</t>
   </si>
@@ -239,6 +240,18 @@
   </si>
   <si>
     <t>seg2</t>
+  </si>
+  <si>
+    <t>theta 1</t>
+  </si>
+  <si>
+    <t>theta 2</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>(nan,nan)</t>
   </si>
 </sst>
 </file>
@@ -628,16 +641,16 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="2"/>
-    <col min="2" max="4" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.06640625" style="2"/>
-    <col min="7" max="7" width="13.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="4" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -773,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -841,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -909,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -977,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1045,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1181,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1249,7 +1262,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1317,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1385,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1453,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1521,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1589,7 +1602,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -1657,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1725,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1793,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1875,14 +1888,14 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +1906,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1918,14 +1931,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>50</v>
@@ -1940,7 +1953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1957,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -1974,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -2025,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2042,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" s="6"/>
     </row>
   </sheetData>
@@ -2059,14 +2072,14 @@
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>57</v>
@@ -2093,7 +2106,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2122,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -2151,7 +2164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -2180,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2209,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2238,14 +2251,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" s="6"/>
     </row>
   </sheetData>
@@ -2257,16 +2270,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C260D1D8-DD7A-4591-9F99-B58043F5F07A}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>55</v>
@@ -2287,7 +2300,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2310,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -2333,7 +2346,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -2356,7 +2369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2379,7 +2392,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2402,7 +2415,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2421,12 +2434,12 @@
       <selection activeCell="D18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
@@ -2434,7 +2447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -2447,7 +2460,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2460,7 +2473,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -2473,7 +2486,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2486,7 +2499,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -2499,7 +2512,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2511,6 +2524,116 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060E0F2E-C580-439D-8ED2-A8B465244D77}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>